<commit_message>
18°  COMMIT  - Aggiornamento della patch  dei TRT di Core
</commit_message>
<xml_diff>
--- a/actionParams/actionsParamsList_AppCore.xlsx
+++ b/actionParams/actionsParamsList_AppCore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorbara\Documents\ArgoX3_API_Mobile_CORE\actionParams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E1FE62-64A4-4410-97B4-3B73A594E25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0E0F84-A900-47DD-ADCA-71F600E39E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26925" yWindow="3450" windowWidth="27000" windowHeight="13200" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="113">
   <si>
     <t>Codice</t>
   </si>
@@ -305,6 +305,69 @@
   </si>
   <si>
     <t>altri parametri</t>
+  </si>
+  <si>
+    <t>PiaveServizi</t>
+  </si>
+  <si>
+    <t>TerreComacar</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>Sito</t>
+  </si>
+  <si>
+    <t>NrMovimento</t>
+  </si>
+  <si>
+    <t>Fam. Movimento</t>
+  </si>
+  <si>
+    <t>Ubic di destinazione</t>
+  </si>
+  <si>
+    <t>Ubicazione</t>
+  </si>
+  <si>
+    <t>Articolo</t>
+  </si>
+  <si>
+    <t>Descrizione1</t>
+  </si>
+  <si>
+    <t>Stato</t>
+  </si>
+  <si>
+    <t>Lotto</t>
+  </si>
+  <si>
+    <t>Quantità UC</t>
+  </si>
+  <si>
+    <t>Matricola</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Unità confezionamento</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Coeff UM-UC</t>
+  </si>
+  <si>
+    <t>YAX3MCSK (Cambio Stock)</t>
   </si>
 </sst>
 </file>
@@ -328,15 +391,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -425,11 +494,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,10 +555,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -747,15 +853,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="59.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="59.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -769,19 +875,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -792,7 +898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -803,10 +909,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -814,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -825,7 +931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -833,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -841,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -852,7 +958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -863,27 +969,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -901,16 +1007,16 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -927,14 +1033,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -942,7 +1048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -953,7 +1059,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
@@ -961,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
@@ -969,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
@@ -980,7 +1086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -988,7 +1094,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -996,7 +1102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -1007,7 +1113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -1018,7 +1124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -1026,7 +1132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -1042,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -1050,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1061,7 +1167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -1069,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
@@ -1088,7 +1194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>40</v>
       </c>
@@ -1096,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1104,7 +1210,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -1112,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>43</v>
       </c>
@@ -1120,7 +1226,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>44</v>
       </c>
@@ -1128,7 +1234,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>45</v>
       </c>
@@ -1136,7 +1242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
@@ -1144,7 +1250,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>47</v>
       </c>
@@ -1155,7 +1261,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>48</v>
       </c>
@@ -1166,7 +1272,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
@@ -1177,7 +1283,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>50</v>
       </c>
@@ -1188,7 +1294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>51</v>
       </c>
@@ -1199,7 +1305,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>52</v>
       </c>
@@ -1210,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>53</v>
       </c>
@@ -1221,7 +1327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>54</v>
       </c>
@@ -1232,7 +1338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>55</v>
       </c>
@@ -1240,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>56</v>
       </c>
@@ -1251,7 +1357,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>57</v>
       </c>
@@ -1262,7 +1368,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>58</v>
       </c>
@@ -1273,7 +1379,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>59</v>
       </c>
@@ -1284,7 +1390,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1401,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>5</v>
       </c>
@@ -1317,7 +1423,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
@@ -1328,7 +1434,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>60</v>
       </c>
@@ -1339,7 +1445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1456,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1478,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>11</v>
       </c>
@@ -1405,7 +1511,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>21</v>
       </c>
@@ -1416,7 +1522,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>20</v>
       </c>
@@ -1427,7 +1533,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>22</v>
       </c>
@@ -1438,7 +1544,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>63</v>
       </c>
@@ -1449,7 +1555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>64</v>
       </c>
@@ -1457,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>65</v>
       </c>
@@ -1468,7 +1574,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>66</v>
       </c>
@@ -1476,7 +1582,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>67</v>
       </c>
@@ -1484,7 +1590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>68</v>
       </c>
@@ -1495,37 +1601,37 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
     </row>
   </sheetData>
@@ -1535,22 +1641,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3203EB5-0BED-476C-91F4-EC5776EF293E}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -1566,6 +1674,230 @@
       <c r="E1" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="F1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1580,16 +1912,16 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -1615,21 +1947,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADDD6E6-69D3-4FB9-B8D1-5B15E1944B96}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -1649,20 +1981,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1682,7 +2014,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1702,7 +2034,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1722,7 +2054,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1742,7 +2074,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1762,7 +2094,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1782,9 +2114,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>